<commit_message>
Se agregan querys para la creación de las bases de datos y tablas
</commit_message>
<xml_diff>
--- a/Diagrama de clases-bases TPC.xlsx
+++ b/Diagrama de clases-bases TPC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/132fbbe32b197521/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/132fbbe32b197521/Desktop/Repositorio GitHub/TPCuatrimestral_EquipoG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9100FFDC-8A27-4AA2-85B2-21099690ABD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C4BF1BF-0194-4663-AFF1-6D8043EB6854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE9BCFD4-4A86-4CD0-A29C-5390188B8A35}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
   <si>
     <t>Clientes</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Cierre</t>
   </si>
   <si>
-    <t>Hereda de Empleado</t>
-  </si>
-  <si>
     <t>Un cliente puede tener varias razones sociales</t>
   </si>
   <si>
@@ -168,7 +165,10 @@
     <t>Codigo</t>
   </si>
   <si>
-    <t>Rz_x_clientes</t>
+    <t>Puesto</t>
+  </si>
+  <si>
+    <t>Puestos</t>
   </si>
 </sst>
 </file>
@@ -249,13 +249,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66695F06-E190-49ED-918B-444E77046F0B}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,40 +602,28 @@
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -644,102 +633,106 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="N7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
@@ -747,7 +740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
@@ -755,31 +748,49 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="H16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="H17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="H18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
@@ -787,7 +798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
@@ -795,26 +806,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="3" t="s">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="5"/>
+      <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="4" t="s">
+    <row r="23" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="3" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="E24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -826,7 +838,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>18</v>
@@ -1024,7 +1036,7 @@
     </row>
     <row r="23" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega página principal
</commit_message>
<xml_diff>
--- a/Diagrama de clases-bases TPC.xlsx
+++ b/Diagrama de clases-bases TPC.xlsx
@@ -249,14 +249,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66695F06-E190-49ED-918B-444E77046F0B}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,14 +701,11 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
-      <c r="E9" s="5"/>
       <c r="I9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E10" s="5"/>
       <c r="I10" s="2" t="s">
         <v>21</v>
       </c>
@@ -719,7 +714,7 @@
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -815,7 +810,6 @@
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
       <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
@@ -824,9 +818,6 @@
       <c r="E23" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="E24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -838,7 +829,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>